<commit_message>
Minor corrections and refactoring. Added logging
</commit_message>
<xml_diff>
--- a/Dispa-SET/Simulation/InputDispa-SET - Config.xlsx
+++ b/Dispa-SET/Simulation/InputDispa-SET - Config.xlsx
@@ -102,12 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,13 +435,13 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>2012</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
@@ -450,13 +449,13 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>2012</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>9</v>
       </c>
     </row>
@@ -464,13 +463,13 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>2012</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>1</v>
       </c>
     </row>
@@ -478,13 +477,13 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>2012</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>9</v>
       </c>
     </row>
@@ -492,13 +491,13 @@
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>3</v>
       </c>
     </row>
@@ -506,13 +505,13 @@
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>1</v>
       </c>
     </row>

</xml_diff>